<commit_message>
setting up github Actions CI
</commit_message>
<xml_diff>
--- a/downloads/processed_template_data.xlsx
+++ b/downloads/processed_template_data.xlsx
@@ -570,7 +570,7 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>2026-02-21 14:37:44</t>
+          <t>2026-02-23 06:27:43</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>2026-02-21 14:37:44</t>
+          <t>2026-02-23 06:27:43</t>
         </is>
       </c>
       <c r="K3" s="2" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>2026-02-21 14:37:44</t>
+          <t>2026-02-23 06:27:43</t>
         </is>
       </c>
       <c r="K4" s="2" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>2026-02-21 14:37:44</t>
+          <t>2026-02-23 06:27:43</t>
         </is>
       </c>
       <c r="K5" s="2" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
-          <t>2026-02-21 14:37:44</t>
+          <t>2026-02-23 06:27:43</t>
         </is>
       </c>
       <c r="K6" s="2" t="inlineStr">

</xml_diff>

<commit_message>
tests file overlap fix
</commit_message>
<xml_diff>
--- a/downloads/processed_template_data.xlsx
+++ b/downloads/processed_template_data.xlsx
@@ -570,7 +570,7 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>2026-02-26 13:26:30</t>
+          <t>2026-02-26 14:28:08</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>2026-02-26 13:26:30</t>
+          <t>2026-02-26 14:28:08</t>
         </is>
       </c>
       <c r="K3" s="2" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>2026-02-26 13:26:30</t>
+          <t>2026-02-26 14:28:08</t>
         </is>
       </c>
       <c r="K4" s="2" t="inlineStr">
@@ -738,7 +738,7 @@
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>2026-02-26 13:26:30</t>
+          <t>2026-02-26 14:28:08</t>
         </is>
       </c>
       <c r="K5" s="2" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
-          <t>2026-02-26 13:26:30</t>
+          <t>2026-02-26 14:28:08</t>
         </is>
       </c>
       <c r="K6" s="2" t="inlineStr">

</xml_diff>